<commit_message>
making a String variable from a SharePoint link and using it as Source for the Excel File
</commit_message>
<xml_diff>
--- a/Excel Files/All Data for PMO Dashboard.xlsx
+++ b/Excel Files/All Data for PMO Dashboard.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CA.Intern\Desktop\PMO-Dashboard\Excel Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rlysam\Documents\PMO Final Folder\Excel Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7072F511-56F6-4243-9CF5-B7AE0AED3265}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9045" firstSheet="6" activeTab="6"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Portfolio Fields" sheetId="1" r:id="rId1"/>
@@ -20,6 +21,7 @@
     <sheet name="Banners and their Bu" sheetId="6" r:id="rId6"/>
     <sheet name="Business Units" sheetId="7" r:id="rId7"/>
     <sheet name="Project Sizes" sheetId="8" r:id="rId8"/>
+    <sheet name="Financial Labels" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="161">
   <si>
     <t>Project Portfolio Fields</t>
   </si>
@@ -507,12 +509,27 @@
   </si>
   <si>
     <t>Weight</t>
+  </si>
+  <si>
+    <t>Financial Labels</t>
+  </si>
+  <si>
+    <t>Total Budget Approved</t>
+  </si>
+  <si>
+    <t>Total Actual Cost</t>
+  </si>
+  <si>
+    <t>Total Cost at Completion</t>
+  </si>
+  <si>
+    <t>Total Savings in PHP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-3409]dd\-mmm\-yy;@"/>
     <numFmt numFmtId="165" formatCode="&quot;₱&quot;#,##0.00"/>
@@ -959,7 +976,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1109,6 +1126,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1498,21 +1516,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection sqref="A1:D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="102" customWidth="1"/>
-    <col min="3" max="4" width="23.7109375" customWidth="1"/>
+    <col min="3" max="4" width="23.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1526,7 +1544,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
@@ -1540,7 +1558,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>8</v>
       </c>
@@ -1554,7 +1572,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>10</v>
       </c>
@@ -1568,7 +1586,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>13</v>
       </c>
@@ -1580,7 +1598,7 @@
       </c>
       <c r="D5" s="12"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>15</v>
       </c>
@@ -1592,7 +1610,7 @@
       </c>
       <c r="D6" s="12"/>
     </row>
-    <row r="7" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>17</v>
       </c>
@@ -1604,7 +1622,7 @@
       </c>
       <c r="D7" s="12"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
         <v>20</v>
       </c>
@@ -1618,7 +1636,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
         <v>23</v>
       </c>
@@ -1630,7 +1648,7 @@
       </c>
       <c r="D9" s="12"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
         <v>25</v>
       </c>
@@ -1642,7 +1660,7 @@
       </c>
       <c r="D10" s="12"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="13" t="s">
         <v>27</v>
       </c>
@@ -1656,7 +1674,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="14" t="s">
         <v>29</v>
       </c>
@@ -1670,7 +1688,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="14" t="s">
         <v>31</v>
       </c>
@@ -1684,7 +1702,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="13" t="s">
         <v>33</v>
       </c>
@@ -1698,7 +1716,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="13" t="s">
         <v>35</v>
       </c>
@@ -1712,7 +1730,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="13" t="s">
         <v>37</v>
       </c>
@@ -1726,7 +1744,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
         <v>39</v>
       </c>
@@ -1740,7 +1758,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
         <v>42</v>
       </c>
@@ -1752,7 +1770,7 @@
       </c>
       <c r="D18" s="12"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
         <v>44</v>
       </c>
@@ -1764,7 +1782,7 @@
       </c>
       <c r="D19" s="12"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
         <v>46</v>
       </c>
@@ -1776,7 +1794,7 @@
       </c>
       <c r="D20" s="12"/>
     </row>
-    <row r="21" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
         <v>48</v>
       </c>
@@ -1788,7 +1806,7 @@
       </c>
       <c r="D21" s="12"/>
     </row>
-    <row r="22" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A22" s="9" t="s">
         <v>50</v>
       </c>
@@ -1800,7 +1818,7 @@
       </c>
       <c r="D22" s="12"/>
     </row>
-    <row r="23" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A23" s="9" t="s">
         <v>52</v>
       </c>
@@ -1812,7 +1830,7 @@
       </c>
       <c r="D23" s="12"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="9" t="s">
         <v>3</v>
       </c>
@@ -1824,7 +1842,7 @@
       </c>
       <c r="D24" s="12"/>
     </row>
-    <row r="25" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A25" s="15" t="s">
         <v>55</v>
       </c>
@@ -1838,7 +1856,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="15" t="s">
         <v>58</v>
       </c>
@@ -1852,7 +1870,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="15" t="s">
         <v>60</v>
       </c>
@@ -1866,7 +1884,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="15" t="s">
         <v>62</v>
       </c>
@@ -1878,7 +1896,7 @@
       </c>
       <c r="D28" s="12"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="15" t="s">
         <v>64</v>
       </c>
@@ -1924,28 +1942,28 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A29"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A29" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="102" customWidth="1"/>
-    <col min="3" max="4" width="23.7109375" customWidth="1"/>
+    <col min="3" max="4" width="23.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
         <v>23</v>
       </c>
@@ -1959,7 +1977,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>67</v>
       </c>
@@ -1971,7 +1989,7 @@
       </c>
       <c r="D2" s="19"/>
     </row>
-    <row r="3" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
         <v>69</v>
       </c>
@@ -1983,7 +2001,7 @@
       </c>
       <c r="D3" s="21"/>
     </row>
-    <row r="4" spans="1:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="42" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="22" t="s">
         <v>71</v>
       </c>
@@ -1995,7 +2013,7 @@
       </c>
       <c r="D4" s="24"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="25" t="s">
         <v>73</v>
       </c>
@@ -2026,21 +2044,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="102" customWidth="1"/>
-    <col min="3" max="4" width="23.7109375" customWidth="1"/>
+    <col min="3" max="4" width="23.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
         <v>25</v>
       </c>
@@ -2054,7 +2072,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="28" t="s">
         <v>75</v>
       </c>
@@ -2066,7 +2084,7 @@
       </c>
       <c r="D2" s="19"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="29" t="s">
         <v>77</v>
       </c>
@@ -2078,7 +2096,7 @@
       </c>
       <c r="D3" s="21"/>
     </row>
-    <row r="4" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="29" t="s">
         <v>79</v>
       </c>
@@ -2107,21 +2125,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="102" customWidth="1"/>
-    <col min="3" max="4" width="23.7109375" customWidth="1"/>
+    <col min="3" max="4" width="23.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
         <v>42</v>
       </c>
@@ -2135,7 +2153,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="30" t="s">
         <v>81</v>
       </c>
@@ -2149,7 +2167,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="31" t="s">
         <v>84</v>
       </c>
@@ -2163,7 +2181,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="31" t="s">
         <v>87</v>
       </c>
@@ -2177,7 +2195,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="32" t="s">
         <v>90</v>
       </c>
@@ -2197,20 +2215,20 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="36" customWidth="1"/>
-    <col min="3" max="6" width="35.5703125" customWidth="1"/>
+    <col min="3" max="6" width="35.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="33" t="s">
         <v>39</v>
       </c>
@@ -2230,7 +2248,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A2" s="37" t="s">
         <v>98</v>
       </c>
@@ -2250,7 +2268,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A3" s="41" t="s">
         <v>104</v>
       </c>
@@ -2270,7 +2288,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="41" t="s">
         <v>109</v>
       </c>
@@ -2290,7 +2308,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="45" t="s">
         <v>115</v>
       </c>
@@ -2316,20 +2334,20 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" customWidth="1"/>
+    <col min="1" max="1" width="18.88671875" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="49" t="s">
         <v>121</v>
       </c>
@@ -2337,7 +2355,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>122</v>
       </c>
@@ -2345,7 +2363,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>123</v>
       </c>
@@ -2353,7 +2371,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>125</v>
       </c>
@@ -2361,7 +2379,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>126</v>
       </c>
@@ -2369,7 +2387,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>128</v>
       </c>
@@ -2377,7 +2395,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>130</v>
       </c>
@@ -2385,7 +2403,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>132</v>
       </c>
@@ -2393,7 +2411,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>134</v>
       </c>
@@ -2401,7 +2419,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>136</v>
       </c>
@@ -2409,7 +2427,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>137</v>
       </c>
@@ -2417,7 +2435,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>138</v>
       </c>
@@ -2425,7 +2443,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>139</v>
       </c>
@@ -2433,7 +2451,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>140</v>
       </c>
@@ -2441,7 +2459,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>142</v>
       </c>
@@ -2449,7 +2467,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>143</v>
       </c>
@@ -2457,7 +2475,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>144</v>
       </c>
@@ -2465,7 +2483,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>145</v>
       </c>
@@ -2473,7 +2491,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>146</v>
       </c>
@@ -2481,7 +2499,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>131</v>
       </c>
@@ -2489,7 +2507,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>147</v>
       </c>
@@ -2497,7 +2515,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>148</v>
       </c>
@@ -2505,7 +2523,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>150</v>
       </c>
@@ -2513,7 +2531,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>151</v>
       </c>
@@ -2526,7 +2544,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0500-000000000000}">
           <x14:formula1>
             <xm:f>'Business Units'!$A$2:$A$11</xm:f>
           </x14:formula1>
@@ -2539,69 +2557,69 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:A11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="49" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>133</v>
       </c>
@@ -2613,64 +2631,105 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="49" t="s">
+        <v>154</v>
+      </c>
+      <c r="B1" s="49" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="50" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="50" t="s">
+        <v>94</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="50" t="s">
+        <v>95</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="50" t="s">
+        <v>96</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="50" t="s">
+        <v>153</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51541AF5-01F9-4AC0-9D51-F5B12FA21899}">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.140625" customWidth="1"/>
+    <col min="1" max="1" width="21.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="49" t="s">
-        <v>154</v>
-      </c>
-      <c r="B1" s="49" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="50" t="s">
-        <v>93</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="50" t="s">
-        <v>94</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="50" t="s">
-        <v>95</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="50" t="s">
-        <v>96</v>
-      </c>
-      <c r="B5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="50" t="s">
-        <v>153</v>
-      </c>
-      <c r="B6">
-        <v>4</v>
+        <v>156</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" s="51" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" s="51" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" s="51" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" s="51" t="s">
+        <v>160</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
before redesign of dashboard (side navigation)
</commit_message>
<xml_diff>
--- a/Excel Files/All Data for PMO Dashboard.xlsx
+++ b/Excel Files/All Data for PMO Dashboard.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rlysam\Documents\PMO Final Folder\Excel Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7072F511-56F6-4243-9CF5-B7AE0AED3265}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC1CE078-DF22-469E-9E1D-F3797CC974C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Portfolio Fields" sheetId="1" r:id="rId1"/>
@@ -19,11 +19,13 @@
     <sheet name="Project Phase" sheetId="4" r:id="rId4"/>
     <sheet name="Proj Sizing Parameters" sheetId="5" r:id="rId5"/>
     <sheet name="Banners and their Bu" sheetId="6" r:id="rId6"/>
-    <sheet name="Business Units" sheetId="7" r:id="rId7"/>
-    <sheet name="Project Sizes" sheetId="8" r:id="rId8"/>
-    <sheet name="Financial Labels" sheetId="9" r:id="rId9"/>
+    <sheet name="Sheet2" sheetId="11" r:id="rId7"/>
+    <sheet name="Sheet1" sheetId="10" r:id="rId8"/>
+    <sheet name="Business Units" sheetId="7" r:id="rId9"/>
+    <sheet name="Project Sizes" sheetId="8" r:id="rId10"/>
+    <sheet name="Financial Labels" sheetId="9" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="162">
   <si>
     <t>Project Portfolio Fields</t>
   </si>
@@ -524,6 +526,9 @@
   </si>
   <si>
     <t>Total Savings in PHP</t>
+  </si>
+  <si>
+    <t>All Banner</t>
   </si>
 </sst>
 </file>
@@ -534,7 +539,7 @@
     <numFmt numFmtId="164" formatCode="[$-3409]dd\-mmm\-yy;@"/>
     <numFmt numFmtId="165" formatCode="&quot;₱&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -611,6 +616,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -650,7 +661,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -968,6 +979,21 @@
         <color indexed="64"/>
       </top>
       <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -1127,7 +1153,9 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1948,6 +1976,113 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="49" t="s">
+        <v>154</v>
+      </c>
+      <c r="B1" s="49" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="50" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="50" t="s">
+        <v>94</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="50" t="s">
+        <v>95</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="50" t="s">
+        <v>96</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="50" t="s">
+        <v>153</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51541AF5-01F9-4AC0-9D51-F5B12FA21899}">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L24" sqref="L24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="49" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" s="50" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" s="50" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" s="50" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" s="50" t="s">
+        <v>160</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D5"/>
@@ -2335,10 +2470,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J37" sqref="J37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2347,7 +2482,7 @@
     <col min="2" max="2" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="49" t="s">
         <v>121</v>
       </c>
@@ -2355,79 +2490,127 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>122</v>
       </c>
       <c r="B2" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D2" t="s">
+        <v>151</v>
+      </c>
+      <c r="F2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>123</v>
       </c>
       <c r="B3" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>131</v>
+      </c>
+      <c r="F3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>125</v>
       </c>
       <c r="B4" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D4" t="s">
+        <v>128</v>
+      </c>
+      <c r="F4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>126</v>
       </c>
       <c r="B5" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D5" t="s">
+        <v>122</v>
+      </c>
+      <c r="F5" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>128</v>
       </c>
       <c r="B6" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>126</v>
+      </c>
+      <c r="F6" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>130</v>
       </c>
       <c r="B7" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D7" t="s">
+        <v>128</v>
+      </c>
+      <c r="F7" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>132</v>
       </c>
       <c r="B8" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D8" t="s">
+        <v>148</v>
+      </c>
+      <c r="F8" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>134</v>
       </c>
       <c r="B9" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D9" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>136</v>
       </c>
       <c r="B10" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D10" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>137</v>
       </c>
@@ -2435,7 +2618,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>138</v>
       </c>
@@ -2443,7 +2626,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>139</v>
       </c>
@@ -2451,7 +2634,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>140</v>
       </c>
@@ -2459,7 +2642,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>142</v>
       </c>
@@ -2467,7 +2650,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>143</v>
       </c>
@@ -2557,6 +2740,197 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{362C1355-43E1-4F6B-821B-4AF9C7A03597}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F2D8E58-2A5C-4456-B958-42B6A3EABD63}">
+  <dimension ref="A1:B20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.88671875" customWidth="1"/>
+    <col min="2" max="2" width="17.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="51" t="s">
+        <v>147</v>
+      </c>
+      <c r="B1" s="51" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="51" t="s">
+        <v>134</v>
+      </c>
+      <c r="B2" s="51" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="51" t="s">
+        <v>151</v>
+      </c>
+      <c r="B3" s="51" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="51" t="s">
+        <v>131</v>
+      </c>
+      <c r="B4" s="51" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="51" t="s">
+        <v>128</v>
+      </c>
+      <c r="B5" s="51" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="51" t="s">
+        <v>122</v>
+      </c>
+      <c r="B6" s="51" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="51" t="s">
+        <v>126</v>
+      </c>
+      <c r="B7" s="51" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="51" t="s">
+        <v>148</v>
+      </c>
+      <c r="B8" s="51" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="51" t="s">
+        <v>143</v>
+      </c>
+      <c r="B9" s="51" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="51" t="s">
+        <v>151</v>
+      </c>
+      <c r="B10" s="51" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="51" t="s">
+        <v>140</v>
+      </c>
+      <c r="B11" s="51" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="51" t="s">
+        <v>122</v>
+      </c>
+      <c r="B12" s="51" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="51" t="s">
+        <v>140</v>
+      </c>
+      <c r="B13" s="51" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="51" t="s">
+        <v>161</v>
+      </c>
+      <c r="B14" s="51" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="51" t="s">
+        <v>147</v>
+      </c>
+      <c r="B15" s="51" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="51" t="s">
+        <v>134</v>
+      </c>
+      <c r="B16" s="51" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="51" t="s">
+        <v>151</v>
+      </c>
+      <c r="B17" s="51" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="51" t="s">
+        <v>131</v>
+      </c>
+      <c r="B18" s="51" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="51" t="s">
+        <v>128</v>
+      </c>
+      <c r="B19" s="51" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="51" t="s">
+        <v>122</v>
+      </c>
+      <c r="B20" s="51" t="s">
+        <v>93</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:A11"/>
   <sheetViews>
@@ -2628,111 +3002,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:B6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="25.109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="49" t="s">
-        <v>154</v>
-      </c>
-      <c r="B1" s="49" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="50" t="s">
-        <v>93</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="50" t="s">
-        <v>94</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="50" t="s">
-        <v>95</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="50" t="s">
-        <v>96</v>
-      </c>
-      <c r="B5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="50" t="s">
-        <v>153</v>
-      </c>
-      <c r="B6">
-        <v>4</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51541AF5-01F9-4AC0-9D51-F5B12FA21899}">
-  <dimension ref="A1:A5"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="21.6640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="49" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" s="51" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" s="51" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" s="51" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" s="51" t="s">
-        <v>160</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>